<commit_message>
Arreglo link de descarga de archivos y formato fecha en excel de Oferta.xlsx
</commit_message>
<xml_diff>
--- a/public/img/oferta.xlsx
+++ b/public/img/oferta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flia. FernCalf\Desktop\Importar archivos\ofertas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cfb\public\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Año</t>
+    <t>Nombre</t>
   </si>
   <si>
-    <t>Fecha de inicio de inscripciones</t>
+    <t>Fecha de inicio de inscripciones (dd/mm/aaaa)</t>
   </si>
   <si>
-    <t>Fecha de fin de inscripciones</t>
+    <t>Fecha de fin de inscripciones (dd/mm/aaaa)</t>
   </si>
   <si>
-    <t>Fecha fin de oferta</t>
+    <t>Fecha fin de oferta (dd/mm/aaaa)</t>
   </si>
   <si>
-    <t>Nombre</t>
+    <t>Año (aaaa)</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -374,10 +376,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>

</xml_diff>